<commit_message>
Update FTSE curve and equity hedge data as of 9/30/22
</commit_message>
<xml_diff>
--- a/data/time_series/equity_hedge_data.xlsx
+++ b/data/time_series/equity_hedge_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70846DF1-33B7-4E39-8B57-1EAB00A641B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B3D6FC-A6CC-4FE3-B342-2E80A3182127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{974027C2-A5EE-46D1-9A10-B8A0BC39505E}"/>
+    <workbookView xWindow="-28920" yWindow="-1485" windowWidth="29040" windowHeight="15840" xr2:uid="{974027C2-A5EE-46D1-9A10-B8A0BC39505E}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Historical Returns" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="20">
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -161,21 +161,6 @@
         <color rgb="FF9C0006"/>
       </font>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
@@ -550,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC31146-373F-4615-8CBA-9FB7E06C62A6}">
-  <dimension ref="A1:ALM177"/>
+  <dimension ref="A1:ALM178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A176" sqref="A176:K177"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A186" sqref="A186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6757,68 +6742,119 @@
         <v>2.7151314716447618E-3</v>
       </c>
     </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A178" s="3">
+        <v>44834</v>
+      </c>
+      <c r="B178" s="2">
+        <v>-9.2098601263658209E-2</v>
+      </c>
+      <c r="C178" s="2">
+        <v>-3.1695302348644587E-2</v>
+      </c>
+      <c r="D178" s="2">
+        <v>1.696093882445959E-3</v>
+      </c>
+      <c r="E178" s="2">
+        <v>3.1942903879981673E-2</v>
+      </c>
+      <c r="F178" s="2">
+        <v>5.3332722001232923E-2</v>
+      </c>
+      <c r="G178" s="2">
+        <v>-1.1989244942036681E-3</v>
+      </c>
+      <c r="H178" s="2">
+        <v>1.0964386230749581E-3</v>
+      </c>
+      <c r="I178" s="2">
+        <v>2.9521574700462241E-3</v>
+      </c>
+      <c r="J178" s="2">
+        <v>-8.7040786056474043E-2</v>
+      </c>
+      <c r="K178" s="2">
+        <v>9.6646150455747919E-3</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A172">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="30">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:K171">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A173:A174">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="26">
       <formula>LEN(TRIM(A173))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172:K174">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A175">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="16">
       <formula>LEN(TRIM(A175))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B175:K175">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A176:A177">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(A176))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B176:K177">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A178">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A178))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B178:K178">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated data to 10/31
</commit_message>
<xml_diff>
--- a/data/time_series/equity_hedge_data.xlsx
+++ b/data/time_series/equity_hedge_data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\time_series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvg9hxp\Documents\Projects\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F102DE7A-3F61-4425-A845-BE9E7DEF72C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B82E7A7-3155-4C55-A98D-DECCA16ABDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{974027C2-A5EE-46D1-9A10-B8A0BC39505E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{974027C2-A5EE-46D1-9A10-B8A0BC39505E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Monthly Historical Returns" sheetId="1" r:id="rId1"/>
+    <sheet name="Monthly Historical Returns" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,9 +45,6 @@
     <t>Down Var</t>
   </si>
   <si>
-    <t>VOLA</t>
-  </si>
-  <si>
     <t>Dynamic Put Spread</t>
   </si>
   <si>
@@ -68,13 +65,16 @@
   <si>
     <t>Weighted Hedges</t>
   </si>
+  <si>
+    <t>VOLA 3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -163,7 +163,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+      <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -474,19 +474,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC31146-373F-4615-8CBA-9FB7E06C62A6}">
-  <dimension ref="A1:ALM172"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D4F897-E655-4325-BF4E-FA224214E13B}">
+  <dimension ref="A1:ALM179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1001" width="21.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1001" width="21.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,31 +497,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>39478</v>
       </c>
@@ -550,13 +550,13 @@
         <v>-2.7100558113250179E-3</v>
       </c>
       <c r="J2" s="2">
-        <v>-5.9101359844524068E-2</v>
+        <v>-5.8734680797807103E-2</v>
       </c>
       <c r="K2" s="2">
         <v>2.301616170161861E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>39507</v>
       </c>
@@ -585,13 +585,13 @@
         <v>1.7484409963956171E-2</v>
       </c>
       <c r="J3" s="2">
-        <v>-2.9374293620508619E-2</v>
+        <v>-2.8077832303431711E-2</v>
       </c>
       <c r="K3" s="2">
-        <v>8.1377879594981186E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.1377879594981203E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>39538</v>
       </c>
@@ -620,13 +620,13 @@
         <v>-4.0243448939915492E-3</v>
       </c>
       <c r="J4" s="2">
-        <v>-5.3524982197180821E-3</v>
+        <v>-5.7835186934232733E-3</v>
       </c>
       <c r="K4" s="2">
         <v>-2.705482358026427E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>39568</v>
       </c>
@@ -655,13 +655,13 @@
         <v>2.1805107250923241E-2</v>
       </c>
       <c r="J5" s="2">
-        <v>4.7493898162789892E-2</v>
+        <v>4.6989950480329112E-2</v>
       </c>
       <c r="K5" s="2">
-        <v>-3.1632408376000461E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.163240837600043E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>39599</v>
       </c>
@@ -690,13 +690,13 @@
         <v>9.0278408396644791E-3</v>
       </c>
       <c r="J6" s="2">
-        <v>1.306345479700069E-2</v>
+        <v>1.3109623518949679E-2</v>
       </c>
       <c r="K6" s="2">
         <v>2.8979751623368818E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>39629</v>
       </c>
@@ -725,13 +725,13 @@
         <v>1.883929737521417E-2</v>
       </c>
       <c r="J7" s="2">
-        <v>-7.9585951395109614E-2</v>
+        <v>-7.7620161609632199E-2</v>
       </c>
       <c r="K7" s="2">
         <v>1.2339111268842811E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>39660</v>
       </c>
@@ -760,13 +760,13 @@
         <v>-3.5884137606431152E-4</v>
       </c>
       <c r="J8" s="2">
-        <v>-8.7038153295425219E-3</v>
+        <v>-8.8278117733593814E-3</v>
       </c>
       <c r="K8" s="2">
         <v>-7.7831613965044641E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>39691</v>
       </c>
@@ -795,13 +795,13 @@
         <v>4.9296313349740384E-3</v>
       </c>
       <c r="J9" s="2">
-        <v>1.604142169957929E-2</v>
+        <v>1.669830734837786E-2</v>
       </c>
       <c r="K9" s="2">
-        <v>4.1232206878433573E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.123220687843359E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>39721</v>
       </c>
@@ -830,13 +830,13 @@
         <v>-4.0317723589338619E-2</v>
       </c>
       <c r="J10" s="2">
-        <v>-7.9957365508925099E-2</v>
+        <v>-7.6144815116839432E-2</v>
       </c>
       <c r="K10" s="2">
         <v>2.393108553801469E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>39752</v>
       </c>
@@ -865,13 +865,13 @@
         <v>2.598813876095197E-3</v>
       </c>
       <c r="J11" s="2">
-        <v>-0.1173761459455574</v>
+        <v>-9.6304716750450992E-2</v>
       </c>
       <c r="K11" s="2">
         <v>0.13226374017851431</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>39782</v>
       </c>
@@ -900,13 +900,13 @@
         <v>-3.6445375733058511E-4</v>
       </c>
       <c r="J12" s="2">
-        <v>-6.907367217661102E-2</v>
+        <v>-6.7956492218953543E-2</v>
       </c>
       <c r="K12" s="2">
-        <v>7.0124526572961634E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.0124526572961608E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>39813</v>
       </c>
@@ -935,13 +935,13 @@
         <v>3.0580629938766511E-2</v>
       </c>
       <c r="J13" s="2">
-        <v>6.4493255317454642E-3</v>
+        <v>4.7031835096489017E-3</v>
       </c>
       <c r="K13" s="2">
         <v>-1.096039915408303E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>39844</v>
       </c>
@@ -970,13 +970,13 @@
         <v>2.158703233295807E-2</v>
       </c>
       <c r="J14" s="2">
-        <v>-8.0643570544795984E-2</v>
+        <v>-7.9125758297121568E-2</v>
       </c>
       <c r="K14" s="2">
         <v>9.5271907238639372E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>39872</v>
       </c>
@@ -1005,13 +1005,13 @@
         <v>1.300845777648141E-2</v>
       </c>
       <c r="J15" s="2">
-        <v>-0.104679673889376</v>
+        <v>-0.10393038505356419</v>
       </c>
       <c r="K15" s="2">
         <v>4.7032283847880307E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>39903</v>
       </c>
@@ -1040,13 +1040,13 @@
         <v>-2.2065098325696358E-3</v>
       </c>
       <c r="J16" s="2">
-        <v>8.77827753155275E-2</v>
+        <v>8.7860818690481124E-2</v>
       </c>
       <c r="K16" s="2">
-        <v>4.8987226124730908E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.8987226124730951E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>39933</v>
       </c>
@@ -1075,13 +1075,13 @@
         <v>3.2042417909272651E-3</v>
       </c>
       <c r="J17" s="2">
-        <v>9.3843378221039248E-2</v>
+        <v>9.3065886188474348E-2</v>
       </c>
       <c r="K17" s="2">
-        <v>-4.8802576813306367E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-4.8802576813306341E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>39964</v>
       </c>
@@ -1110,13 +1110,13 @@
         <v>1.402443726635103E-2</v>
       </c>
       <c r="J18" s="2">
-        <v>5.9562350841644497E-2</v>
+        <v>6.107451897661053E-2</v>
       </c>
       <c r="K18" s="2">
         <v>9.4917630625560127E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>39994</v>
       </c>
@@ -1145,13 +1145,13 @@
         <v>1.7937744633358382E-2</v>
       </c>
       <c r="J19" s="2">
-        <v>3.9080107559120707E-3</v>
+        <v>4.7096825994103536E-3</v>
       </c>
       <c r="K19" s="2">
-        <v>5.0320324945738416E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.0320324945738407E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>40025</v>
       </c>
@@ -1180,13 +1180,13 @@
         <v>1.317936303442482E-2</v>
       </c>
       <c r="J20" s="2">
-        <v>7.7914491427940741E-2</v>
+        <v>7.8863473394695446E-2</v>
       </c>
       <c r="K20" s="2">
         <v>5.9566868067064153E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>40056</v>
       </c>
@@ -1215,13 +1215,13 @@
         <v>1.6708794857041132E-2</v>
       </c>
       <c r="J21" s="2">
-        <v>3.9324707603011967E-2</v>
+        <v>4.0666646478373251E-2</v>
       </c>
       <c r="K21" s="2">
         <v>8.4232470945753857E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>40086</v>
       </c>
@@ -1250,13 +1250,13 @@
         <v>2.881421741962216E-2</v>
       </c>
       <c r="J22" s="2">
-        <v>3.7714789185809873E-2</v>
+        <v>3.7881259700095621E-2</v>
       </c>
       <c r="K22" s="2">
-        <v>1.044922612747473E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.0449226127474741E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>40117</v>
       </c>
@@ -1285,13 +1285,13 @@
         <v>1.8859043939336701E-2</v>
       </c>
       <c r="J23" s="2">
-        <v>-1.547025087779874E-2</v>
+        <v>-1.417584941607454E-2</v>
       </c>
       <c r="K23" s="2">
         <v>8.1248584058996372E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>40147</v>
       </c>
@@ -1320,13 +1320,13 @@
         <v>5.6246510277788717E-3</v>
       </c>
       <c r="J24" s="2">
-        <v>6.0546521960695217E-2</v>
+        <v>6.0781119093961777E-2</v>
       </c>
       <c r="K24" s="2">
         <v>1.472548159580891E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>40178</v>
       </c>
@@ -1355,13 +1355,13 @@
         <v>2.2748521455544731E-2</v>
       </c>
       <c r="J25" s="2">
-        <v>2.175538858707227E-2</v>
+        <v>2.2772162662833429E-2</v>
       </c>
       <c r="K25" s="2">
-        <v>6.3822126601623197E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.3822126601623189E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>40209</v>
       </c>
@@ -1390,13 +1390,13 @@
         <v>3.7746357383442891E-3</v>
       </c>
       <c r="J26" s="2">
-        <v>-3.4550548699807733E-2</v>
+        <v>-3.3957713611949172E-2</v>
       </c>
       <c r="K26" s="2">
         <v>3.721180243789114E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>40237</v>
       </c>
@@ -1425,13 +1425,13 @@
         <v>3.1629608710803002E-3</v>
       </c>
       <c r="J27" s="2">
-        <v>2.8408230908076058E-2</v>
+        <v>2.7337815388362309E-2</v>
       </c>
       <c r="K27" s="2">
         <v>-6.718915877587852E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>40268</v>
       </c>
@@ -1460,13 +1460,13 @@
         <v>2.327016740919579E-2</v>
       </c>
       <c r="J28" s="2">
-        <v>6.0233214751433638E-2</v>
+        <v>6.0186711370435672E-2</v>
       </c>
       <c r="K28" s="2">
-        <v>-2.9189814534110012E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-2.918981453410999E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>40298</v>
       </c>
@@ -1495,13 +1495,13 @@
         <v>4.381510937907329E-3</v>
       </c>
       <c r="J29" s="2">
-        <v>1.944319182924412E-2</v>
+        <v>2.0966424867023398E-2</v>
       </c>
       <c r="K29" s="2">
-        <v>9.5612166063684199E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.5612166063684181E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>40329</v>
       </c>
@@ -1530,13 +1530,13 @@
         <v>-1.410911974086085E-2</v>
       </c>
       <c r="J30" s="2">
-        <v>-8.1650400214249755E-2</v>
+        <v>-8.2400326053040068E-2</v>
       </c>
       <c r="K30" s="2">
-        <v>-4.7072268034837033E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-4.707226803483705E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>40359</v>
       </c>
@@ -1565,13 +1565,13 @@
         <v>2.2504359779677841E-2</v>
       </c>
       <c r="J31" s="2">
-        <v>-4.9164805114291277E-2</v>
+        <v>-4.7838193220810683E-2</v>
       </c>
       <c r="K31" s="2">
-        <v>8.3270408083089796E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.3270408083089813E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>40390</v>
       </c>
@@ -1600,13 +1600,13 @@
         <v>1.170879997086245E-2</v>
       </c>
       <c r="J32" s="2">
-        <v>6.7941557135837966E-2</v>
+        <v>6.7057401410991674E-2</v>
       </c>
       <c r="K32" s="2">
-        <v>-5.549777472881481E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-5.5497774728814819E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>40421</v>
       </c>
@@ -1635,13 +1635,13 @@
         <v>1.267296837086189E-2</v>
       </c>
       <c r="J33" s="2">
-        <v>-4.2583688876611153E-2</v>
+        <v>-4.151677411263361E-2</v>
       </c>
       <c r="K33" s="2">
-        <v>6.696941903120604E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.6969419031206049E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>40451</v>
       </c>
@@ -1670,13 +1670,13 @@
         <v>2.040706743879284E-2</v>
       </c>
       <c r="J34" s="2">
-        <v>9.2251941413481003E-2</v>
+        <v>9.3505063755783449E-2</v>
       </c>
       <c r="K34" s="2">
         <v>7.8657525486060653E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>40482</v>
       </c>
@@ -1705,13 +1705,13 @@
         <v>1.694596149221057E-2</v>
       </c>
       <c r="J35" s="2">
-        <v>3.6056146584614729E-2</v>
+        <v>3.5225720406146091E-2</v>
       </c>
       <c r="K35" s="2">
-        <v>-5.2125212433108137E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-5.2125212433108154E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>40512</v>
       </c>
@@ -1740,13 +1740,13 @@
         <v>9.5955329345957206E-3</v>
       </c>
       <c r="J36" s="2">
-        <v>2.9045826680546461E-3</v>
+        <v>4.0614170216733414E-3</v>
       </c>
       <c r="K36" s="2">
         <v>7.2613602504065788E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>40543</v>
       </c>
@@ -1775,13 +1775,13 @@
         <v>2.5901549267020069E-2</v>
       </c>
       <c r="J37" s="2">
-        <v>6.7972684802329666E-2</v>
+        <v>6.844802565072941E-2</v>
       </c>
       <c r="K37" s="2">
         <v>2.983677940724622E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>40574</v>
       </c>
@@ -1810,13 +1810,13 @@
         <v>1.8462896675959749E-2</v>
       </c>
       <c r="J38" s="2">
-        <v>2.526669942377064E-2</v>
+        <v>2.5918830521976119E-2</v>
       </c>
       <c r="K38" s="2">
         <v>4.0933767395051578E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>40602</v>
       </c>
@@ -1845,13 +1845,13 @@
         <v>2.1678636516189509E-2</v>
       </c>
       <c r="J39" s="2">
-        <v>3.4528213208327052E-2</v>
+        <v>3.4640426548244951E-2</v>
       </c>
       <c r="K39" s="2">
         <v>7.0435450286933203E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>40633</v>
       </c>
@@ -1880,13 +1880,13 @@
         <v>6.964290471221735E-3</v>
       </c>
       <c r="J40" s="2">
-        <v>6.4356331401477663E-4</v>
+        <v>7.4605693975588979E-4</v>
       </c>
       <c r="K40" s="2">
-        <v>6.4334460465191113E-4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.4334460465191123E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40663</v>
       </c>
@@ -1915,13 +1915,13 @@
         <v>1.691585366878923E-2</v>
       </c>
       <c r="J41" s="2">
-        <v>3.063232599802123E-2</v>
+        <v>3.1056034184821401E-2</v>
       </c>
       <c r="K41" s="2">
         <v>2.659583695607219E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>40694</v>
       </c>
@@ -1950,13 +1950,13 @@
         <v>9.2176153622681722E-3</v>
       </c>
       <c r="J42" s="2">
-        <v>-1.027185903737469E-2</v>
+        <v>-9.8353571992980757E-3</v>
       </c>
       <c r="K42" s="2">
         <v>2.7398884605424321E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>40724</v>
       </c>
@@ -1985,13 +1985,13 @@
         <v>9.3065807311118551E-3</v>
       </c>
       <c r="J43" s="2">
-        <v>-1.6604482929331602E-2</v>
+        <v>-1.6577546449416371E-2</v>
       </c>
       <c r="K43" s="2">
-        <v>1.6907821239101761E-4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.6907821239101731E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>40755</v>
       </c>
@@ -2020,13 +2020,13 @@
         <v>6.5263392833909478E-3</v>
       </c>
       <c r="J44" s="2">
-        <v>-1.9316386562916388E-2</v>
+        <v>-1.889200465162013E-2</v>
       </c>
       <c r="K44" s="2">
         <v>2.663812612444165E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>40786</v>
       </c>
@@ -2055,13 +2055,13 @@
         <v>5.9707382909908726E-3</v>
       </c>
       <c r="J45" s="2">
-        <v>-4.5723911600821267E-2</v>
+        <v>-4.2141451312966573E-2</v>
       </c>
       <c r="K45" s="2">
-        <v>2.2486827652995641E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.2486827652995652E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>40816</v>
       </c>
@@ -2090,13 +2090,13 @@
         <v>1.6597288924616489E-2</v>
       </c>
       <c r="J46" s="2">
-        <v>-6.4964464294628252E-2</v>
+        <v>-6.274190929606141E-2</v>
       </c>
       <c r="K46" s="2">
         <v>1.395080676023509E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>40847</v>
       </c>
@@ -2125,13 +2125,13 @@
         <v>1.553627295097388E-2</v>
       </c>
       <c r="J47" s="2">
-        <v>0.1072582322137285</v>
+        <v>0.10641035234823309</v>
       </c>
       <c r="K47" s="2">
-        <v>-5.3220766941861368E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-5.3220766941861359E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>40877</v>
       </c>
@@ -2160,13 +2160,13 @@
         <v>4.5049312797990522E-3</v>
       </c>
       <c r="J48" s="2">
-        <v>1.2071910137528099E-4</v>
+        <v>1.0919683345467441E-3</v>
       </c>
       <c r="K48" s="2">
         <v>6.0964567251378006E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>40908</v>
       </c>
@@ -2195,13 +2195,13 @@
         <v>1.515375246371398E-2</v>
       </c>
       <c r="J49" s="2">
-        <v>9.3419863051493642E-3</v>
+        <v>8.972233613944192E-3</v>
       </c>
       <c r="K49" s="2">
-        <v>-2.3209092001801618E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-2.3209092001801632E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>40939</v>
       </c>
@@ -2230,13 +2230,13 @@
         <v>1.352884835728585E-2</v>
       </c>
       <c r="J50" s="2">
-        <v>4.3491923017074448E-2</v>
+        <v>4.2940603590315568E-2</v>
       </c>
       <c r="K50" s="2">
-        <v>-3.4605896325788249E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.460589632578824E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>40968</v>
       </c>
@@ -2265,13 +2265,13 @@
         <v>2.4000526429026621E-2</v>
       </c>
       <c r="J51" s="2">
-        <v>4.6279992108088239E-2</v>
+        <v>4.7545746459763893E-2</v>
       </c>
       <c r="K51" s="2">
         <v>7.9450426997486959E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>40999</v>
       </c>
@@ -2300,13 +2300,13 @@
         <v>1.229630121568788E-2</v>
       </c>
       <c r="J52" s="2">
-        <v>3.07751478790852E-2</v>
+        <v>2.9885956402886209E-2</v>
       </c>
       <c r="K52" s="2">
         <v>-5.5813864967567597E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>41029</v>
       </c>
@@ -2335,13 +2335,13 @@
         <v>2.1060019626575351E-4</v>
       </c>
       <c r="J53" s="2">
-        <v>-6.2131295370382684E-3</v>
+        <v>-6.186576322643151E-3</v>
       </c>
       <c r="K53" s="2">
-        <v>1.6667248420320629E-4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.6667248420320599E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>41060</v>
       </c>
@@ -2370,13 +2370,13 @@
         <v>1.082277679991916E-2</v>
       </c>
       <c r="J54" s="2">
-        <v>-6.0740126575994161E-2</v>
+        <v>-6.1006608239129123E-2</v>
       </c>
       <c r="K54" s="2">
         <v>-1.67268490090864E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>41090</v>
       </c>
@@ -2405,13 +2405,13 @@
         <v>1.128498227616785E-2</v>
       </c>
       <c r="J55" s="2">
-        <v>4.1958853662789383E-2</v>
+        <v>4.2274180082043353E-2</v>
       </c>
       <c r="K55" s="2">
         <v>1.9792796777787802E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>41121</v>
       </c>
@@ -2440,13 +2440,13 @@
         <v>-7.7278726130378702E-4</v>
       </c>
       <c r="J56" s="2">
-        <v>1.27193014565724E-2</v>
+        <v>1.223186808701375E-2</v>
       </c>
       <c r="K56" s="2">
-        <v>-3.0595817658450892E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.0595817658450901E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>41152</v>
       </c>
@@ -2475,13 +2475,13 @@
         <v>1.5713771995621451E-2</v>
       </c>
       <c r="J57" s="2">
-        <v>2.3839671839735E-2</v>
+        <v>2.438847152508106E-2</v>
       </c>
       <c r="K57" s="2">
-        <v>3.4447734095568732E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.4447734095568719E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>41182</v>
       </c>
@@ -2510,13 +2510,13 @@
         <v>1.286497964114721E-2</v>
       </c>
       <c r="J58" s="2">
-        <v>2.5201431588669981E-2</v>
+        <v>2.4934588191046811E-2</v>
       </c>
       <c r="K58" s="2">
         <v>-1.674955480465451E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>41213</v>
       </c>
@@ -2545,13 +2545,13 @@
         <v>1.5874883472192729E-2</v>
       </c>
       <c r="J59" s="2">
-        <v>-1.8130810875045911E-2</v>
+        <v>-1.799183782052555E-2</v>
       </c>
       <c r="K59" s="2">
-        <v>8.7232317298933416E-4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.723231729893346E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>41243</v>
       </c>
@@ -2580,13 +2580,13 @@
         <v>1.08650755573181E-2</v>
       </c>
       <c r="J60" s="2">
-        <v>7.2961604138800191E-3</v>
+        <v>7.9191462681866102E-3</v>
       </c>
       <c r="K60" s="2">
         <v>3.9104342854936799E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>41274</v>
       </c>
@@ -2615,13 +2615,13 @@
         <v>1.6380343072573061E-2</v>
       </c>
       <c r="J61" s="2">
-        <v>1.19838985003864E-2</v>
+        <v>1.317940844966729E-2</v>
       </c>
       <c r="K61" s="2">
         <v>7.5041239893324056E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>41305</v>
       </c>
@@ -2650,13 +2650,13 @@
         <v>9.3789371295559948E-3</v>
       </c>
       <c r="J62" s="2">
-        <v>5.1362592721517983E-2</v>
+        <v>5.1182360663807068E-2</v>
       </c>
       <c r="K62" s="2">
         <v>-1.131302762246995E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>41333</v>
       </c>
@@ -2685,13 +2685,13 @@
         <v>-4.8524361902499537E-3</v>
       </c>
       <c r="J63" s="2">
-        <v>1.461687104778189E-2</v>
+        <v>1.5051100336237249E-2</v>
       </c>
       <c r="K63" s="2">
         <v>2.72562384138131E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>41364</v>
       </c>
@@ -2720,13 +2720,13 @@
         <v>9.069685695920638E-3</v>
       </c>
       <c r="J64" s="2">
-        <v>3.8576047947432267E-2</v>
+        <v>3.9022990869633338E-2</v>
       </c>
       <c r="K64" s="2">
         <v>2.805426342431265E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>41394</v>
       </c>
@@ -2755,13 +2755,13 @@
         <v>-2.333309587484299E-3</v>
       </c>
       <c r="J65" s="2">
-        <v>1.9244667311573309E-2</v>
+        <v>1.9235595677250202E-2</v>
       </c>
       <c r="K65" s="2">
-        <v>-5.6941950828121989E-5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-5.6941950828121942E-5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>41425</v>
       </c>
@@ -2790,13 +2790,13 @@
         <v>6.2462276122290342E-4</v>
       </c>
       <c r="J66" s="2">
-        <v>2.3143564974501329E-2</v>
+        <v>2.304011195600696E-2</v>
       </c>
       <c r="K66" s="2">
         <v>-6.4936663916470821E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>41455</v>
       </c>
@@ -2825,13 +2825,13 @@
         <v>2.112834878646041E-3</v>
       </c>
       <c r="J67" s="2">
-        <v>-1.2609042569417641E-2</v>
+        <v>-1.226748189974552E-2</v>
       </c>
       <c r="K67" s="2">
         <v>2.143950049634232E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>41486</v>
       </c>
@@ -2860,13 +2860,13 @@
         <v>1.504422083575181E-2</v>
       </c>
       <c r="J68" s="2">
-        <v>5.122494284926938E-2</v>
+        <v>5.1366868659336172E-2</v>
       </c>
       <c r="K68" s="2">
         <v>8.908573924192283E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>41517</v>
       </c>
@@ -2895,13 +2895,13 @@
         <v>1.1715847817497901E-2</v>
       </c>
       <c r="J69" s="2">
-        <v>-2.7568082913479869E-2</v>
+        <v>-2.6987413032617528E-2</v>
       </c>
       <c r="K69" s="2">
         <v>3.6448201752590221E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>41547</v>
       </c>
@@ -2930,13 +2930,13 @@
         <v>8.3014773985466955E-3</v>
       </c>
       <c r="J70" s="2">
-        <v>3.0732641528178482E-2</v>
+        <v>3.047136087879895E-2</v>
       </c>
       <c r="K70" s="2">
         <v>-1.640038537643779E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>41578</v>
       </c>
@@ -2965,13 +2965,13 @@
         <v>1.439162768615836E-2</v>
       </c>
       <c r="J71" s="2">
-        <v>4.6263031716124323E-2</v>
+        <v>4.6386132180997977E-2</v>
       </c>
       <c r="K71" s="2">
-        <v>7.7269214874543042E-4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.7269214874543064E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>41608</v>
       </c>
@@ -3000,13 +3000,13 @@
         <v>9.9920275671750991E-3</v>
       </c>
       <c r="J72" s="2">
-        <v>3.1368002559812411E-2</v>
+        <v>3.1740524161715987E-2</v>
       </c>
       <c r="K72" s="2">
         <v>2.3382894396408891E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>41639</v>
       </c>
@@ -3035,13 +3035,13 @@
         <v>1.5538063340502759E-2</v>
       </c>
       <c r="J73" s="2">
-        <v>2.63044673815391E-2</v>
+        <v>2.6716310174183251E-2</v>
       </c>
       <c r="K73" s="2">
         <v>2.5851055292125261E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>41670</v>
       </c>
@@ -3070,13 +3070,13 @@
         <v>6.670833381218589E-3</v>
       </c>
       <c r="J74" s="2">
-        <v>-3.4607086432201027E-2</v>
+        <v>-3.4620876943316142E-2</v>
       </c>
       <c r="K74" s="2">
-        <v>-8.6561977460945815E-5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-8.6561977460945707E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>41698</v>
       </c>
@@ -3105,13 +3105,13 @@
         <v>9.2507655101985668E-3</v>
       </c>
       <c r="J75" s="2">
-        <v>4.5415646113015143E-2</v>
+        <v>4.5278877329950527E-2</v>
       </c>
       <c r="K75" s="2">
         <v>-8.584871306209405E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>41729</v>
       </c>
@@ -3140,13 +3140,13 @@
         <v>1.4153374329733339E-2</v>
       </c>
       <c r="J76" s="2">
-        <v>9.4991513007536381E-3</v>
+        <v>9.9547607946417274E-3</v>
       </c>
       <c r="K76" s="2">
         <v>2.859825746251383E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>41759</v>
       </c>
@@ -3175,13 +3175,13 @@
         <v>7.1655190744856819E-3</v>
       </c>
       <c r="J77" s="2">
-        <v>6.9406875104919899E-3</v>
+        <v>6.7526149766039614E-3</v>
       </c>
       <c r="K77" s="2">
         <v>-1.180516828097175E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>41790</v>
       </c>
@@ -3210,13 +3210,13 @@
         <v>6.5936928846640928E-3</v>
       </c>
       <c r="J78" s="2">
-        <v>2.31441384472021E-2</v>
+        <v>2.30066367556277E-2</v>
       </c>
       <c r="K78" s="2">
-        <v>-8.6308754095930286E-4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-8.6308754095930297E-4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>41820</v>
       </c>
@@ -3245,13 +3245,13 @@
         <v>1.362368243270775E-2</v>
       </c>
       <c r="J79" s="2">
-        <v>2.001081848151277E-2</v>
+        <v>1.9741373758282391E-2</v>
       </c>
       <c r="K79" s="2">
         <v>-1.691283801199904E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>41851</v>
       </c>
@@ -3280,13 +3280,13 @@
         <v>4.6672531882057337E-3</v>
       </c>
       <c r="J80" s="2">
-        <v>-1.2812703353457921E-2</v>
+        <v>-1.2405096402703569E-2</v>
       </c>
       <c r="K80" s="2">
         <v>2.5585174755042412E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>41882</v>
       </c>
@@ -3315,13 +3315,13 @@
         <v>1.6986525278803979E-2</v>
       </c>
       <c r="J81" s="2">
-        <v>4.0173426556449468E-2</v>
+        <v>4.0243637111920923E-2</v>
       </c>
       <c r="K81" s="2">
         <v>4.4070625588232609E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>41912</v>
       </c>
@@ -3350,13 +3350,13 @@
         <v>1.2142521122817751E-2</v>
       </c>
       <c r="J82" s="2">
-        <v>-1.414560859418103E-2</v>
+        <v>-1.419641449296361E-2</v>
       </c>
       <c r="K82" s="2">
-        <v>-3.1890471851218959E-4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.1890471851218948E-4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>41943</v>
       </c>
@@ -3385,13 +3385,13 @@
         <v>7.9839746163550256E-4</v>
       </c>
       <c r="J83" s="2">
-        <v>2.5728457620245809E-2</v>
+        <v>2.627140356693412E-2</v>
       </c>
       <c r="K83" s="2">
-        <v>3.4080299422896789E-3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.4080299422896798E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>41973</v>
       </c>
@@ -3420,13 +3420,13 @@
         <v>1.557029282997484E-2</v>
       </c>
       <c r="J84" s="2">
-        <v>2.7434869977413779E-2</v>
+        <v>2.765996041910844E-2</v>
       </c>
       <c r="K84" s="2">
-        <v>1.4128753878679969E-3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.412875387867998E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>42004</v>
       </c>
@@ -3455,13 +3455,13 @@
         <v>-1.7612718332473459E-3</v>
       </c>
       <c r="J85" s="2">
-        <v>-1.468063874674066E-3</v>
+        <v>-1.030085641226939E-3</v>
       </c>
       <c r="K85" s="2">
         <v>2.749155680714278E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>42035</v>
       </c>
@@ -3490,13 +3490,13 @@
         <v>-1.9469878782717449E-4</v>
       </c>
       <c r="J86" s="2">
-        <v>-2.828928593265264E-2</v>
+        <v>-2.756844123224382E-2</v>
       </c>
       <c r="K86" s="2">
-        <v>4.5246867348738588E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.5246867348738597E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>42063</v>
       </c>
@@ -3525,13 +3525,13 @@
         <v>1.0301245302461371E-2</v>
       </c>
       <c r="J87" s="2">
-        <v>5.6093661752420212E-2</v>
+        <v>5.5519462871669721E-2</v>
       </c>
       <c r="K87" s="2">
         <v>-3.604202205326141E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>42094</v>
       </c>
@@ -3560,13 +3560,13 @@
         <v>-7.660311697473166E-4</v>
       </c>
       <c r="J88" s="2">
-        <v>-1.518563636596046E-2</v>
+        <v>-1.492355075814494E-2</v>
       </c>
       <c r="K88" s="2">
         <v>1.645091199826626E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>42124</v>
       </c>
@@ -3595,13 +3595,13 @@
         <v>8.3813677004296316E-3</v>
       </c>
       <c r="J89" s="2">
-        <v>9.1480282924756504E-3</v>
+        <v>8.9625100521779008E-3</v>
       </c>
       <c r="K89" s="2">
         <v>-1.164483723715108E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>42155</v>
       </c>
@@ -3630,13 +3630,13 @@
         <v>1.0016090430947199E-3</v>
       </c>
       <c r="J90" s="2">
-        <v>1.0448468419482109E-2</v>
+        <v>9.4440149248314776E-3</v>
       </c>
       <c r="K90" s="2">
-        <v>-6.3048773202685707E-3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-6.3048773202685716E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>42185</v>
       </c>
@@ -3665,13 +3665,13 @@
         <v>1.920208342308212E-2</v>
       </c>
       <c r="J91" s="2">
-        <v>-1.874478082982586E-2</v>
+        <v>-1.84893182145459E-2</v>
       </c>
       <c r="K91" s="2">
         <v>1.6035191851419129E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>42216</v>
       </c>
@@ -3700,13 +3700,13 @@
         <v>6.611956050830114E-3</v>
       </c>
       <c r="J92" s="2">
-        <v>2.09875644633962E-2</v>
+        <v>2.1002683496670459E-2</v>
       </c>
       <c r="K92" s="2">
         <v>9.4901008859985328E-5</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>42247</v>
       </c>
@@ -3735,13 +3735,13 @@
         <v>-2.8547169737788359E-2</v>
       </c>
       <c r="J93" s="2">
-        <v>-5.4476201745776068E-2</v>
+        <v>-5.2035473564272343E-2</v>
       </c>
       <c r="K93" s="2">
         <v>1.532026304697728E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>42277</v>
       </c>
@@ -3770,13 +3770,13 @@
         <v>1.3941455847165621E-2</v>
       </c>
       <c r="J94" s="2">
-        <v>-2.5530051210396809E-2</v>
+        <v>-2.5857757248778809E-2</v>
       </c>
       <c r="K94" s="2">
         <v>-2.0569855947670541E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>42308</v>
       </c>
@@ -3805,13 +3805,13 @@
         <v>4.7321219236691843E-3</v>
       </c>
       <c r="J95" s="2">
-        <v>8.3759115467530731E-2</v>
+        <v>8.3511154075278718E-2</v>
       </c>
       <c r="K95" s="2">
         <v>-1.556434585212629E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>42338</v>
       </c>
@@ -3840,13 +3840,13 @@
         <v>5.6263385851517116E-3</v>
       </c>
       <c r="J96" s="2">
-        <v>3.6077837796653382E-3</v>
+        <v>3.8718964553835561E-3</v>
       </c>
       <c r="K96" s="2">
         <v>1.657814949123583E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>42369</v>
       </c>
@@ -3875,13 +3875,13 @@
         <v>3.7605389643311391E-3</v>
       </c>
       <c r="J97" s="2">
-        <v>-1.7035106269916521E-2</v>
+        <v>-1.7561421989094619E-2</v>
       </c>
       <c r="K97" s="2">
-        <v>-3.3036432834563901E-3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.3036432834563909E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>42400</v>
       </c>
@@ -3910,13 +3910,13 @@
         <v>-1.016012191042393E-3</v>
       </c>
       <c r="J98" s="2">
-        <v>-4.8462515859880498E-2</v>
+        <v>-4.7978479884844501E-2</v>
       </c>
       <c r="K98" s="2">
         <v>3.0382565817643902E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>42429</v>
       </c>
@@ -3945,13 +3945,13 @@
         <v>-7.8570650260103572E-4</v>
       </c>
       <c r="J99" s="2">
-        <v>-1.240495282436733E-3</v>
+        <v>-1.1952290782459071E-3</v>
       </c>
       <c r="K99" s="2">
-        <v>2.841324816901076E-4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.8413248169010749E-4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>42460</v>
       </c>
@@ -3980,13 +3980,13 @@
         <v>1.457240383036278E-2</v>
       </c>
       <c r="J100" s="2">
-        <v>6.7306845343063332E-2</v>
+        <v>6.7085465243645545E-2</v>
       </c>
       <c r="K100" s="2">
         <v>-1.3895858548069889E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>42490</v>
       </c>
@@ -4015,13 +4015,13 @@
         <v>2.6751539797304049E-3</v>
       </c>
       <c r="J101" s="2">
-        <v>3.852511351715859E-3</v>
+        <v>3.842421268520422E-3</v>
       </c>
       <c r="K101" s="2">
-        <v>-6.3334676057508654E-5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-6.3334676057508709E-5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>42521</v>
       </c>
@@ -4050,13 +4050,13 @@
         <v>1.540839450619314E-3</v>
       </c>
       <c r="J102" s="2">
-        <v>1.70507573166029E-2</v>
+        <v>1.6672737888603621E-2</v>
       </c>
       <c r="K102" s="2">
         <v>-2.3727988711340041E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>42551</v>
       </c>
@@ -4085,13 +4085,13 @@
         <v>1.709579980714385E-2</v>
       </c>
       <c r="J103" s="2">
-        <v>3.476059882988838E-3</v>
+        <v>3.8447346613752868E-3</v>
       </c>
       <c r="K103" s="2">
         <v>2.3141432243333998E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>42582</v>
       </c>
@@ -4120,13 +4120,13 @@
         <v>7.493221968924677E-3</v>
       </c>
       <c r="J104" s="2">
-        <v>3.5537986226600052E-2</v>
+        <v>3.4983584793088301E-2</v>
       </c>
       <c r="K104" s="2">
-        <v>-3.4799351518891258E-3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.4799351518891271E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>42613</v>
       </c>
@@ -4155,13 +4155,13 @@
         <v>1.018050780520412E-2</v>
       </c>
       <c r="J105" s="2">
-        <v>2.373981735892225E-3</v>
+        <v>2.7781174231747609E-3</v>
       </c>
       <c r="K105" s="2">
-        <v>2.5367286217119161E-3</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.5367286217119148E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>42643</v>
       </c>
@@ -4190,13 +4190,13 @@
         <v>3.3264412176906548E-4</v>
       </c>
       <c r="J106" s="2">
-        <v>-6.6884450850634828E-4</v>
+        <v>-1.026306633469732E-3</v>
       </c>
       <c r="K106" s="2">
         <v>-2.2437622613086278E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>42674</v>
       </c>
@@ -4225,13 +4225,13 @@
         <v>1.181811401525064E-2</v>
       </c>
       <c r="J107" s="2">
-        <v>-1.8478562682408169E-2</v>
+        <v>-1.857747923266231E-2</v>
       </c>
       <c r="K107" s="2">
-        <v>-6.2089157697984361E-4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-6.2089157697984296E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>42704</v>
       </c>
@@ -4260,13 +4260,13 @@
         <v>1.5841909601487261E-2</v>
       </c>
       <c r="J108" s="2">
-        <v>3.827124229440871E-2</v>
+        <v>3.8786402279952052E-2</v>
       </c>
       <c r="K108" s="2">
         <v>3.233619601564357E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>42735</v>
       </c>
@@ -4295,13 +4295,13 @@
         <v>5.6986444530973566E-3</v>
       </c>
       <c r="J109" s="2">
-        <v>1.9908621101799619E-2</v>
+        <v>1.9967927310676811E-2</v>
       </c>
       <c r="K109" s="2">
-        <v>3.7226051110603582E-4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.7226051110603588E-4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>42766</v>
       </c>
@@ -4330,13 +4330,13 @@
         <v>4.5821002135177924E-3</v>
       </c>
       <c r="J110" s="2">
-        <v>1.7537211763433921E-2</v>
+        <v>1.6941702338897531E-2</v>
       </c>
       <c r="K110" s="2">
         <v>-3.7379668493976552E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>42794</v>
       </c>
@@ -4365,13 +4365,13 @@
         <v>7.0743753119562056E-3</v>
       </c>
       <c r="J111" s="2">
-        <v>4.0758800945788688E-2</v>
+        <v>4.1197545837626928E-2</v>
       </c>
       <c r="K111" s="2">
         <v>2.7539679364615511E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>42825</v>
       </c>
@@ -4400,13 +4400,13 @@
         <v>4.5546557439132716E-3</v>
       </c>
       <c r="J112" s="2">
-        <v>-1.389846733654938E-4</v>
+        <v>-6.829681480272781E-4</v>
       </c>
       <c r="K112" s="2">
         <v>-3.4145424255693549E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>42855</v>
       </c>
@@ -4435,13 +4435,13 @@
         <v>9.1970001713444615E-3</v>
       </c>
       <c r="J113" s="2">
-        <v>9.1740381270550529E-3</v>
+        <v>8.717428433869032E-3</v>
       </c>
       <c r="K113" s="2">
         <v>-2.8661039203060948E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>42886</v>
       </c>
@@ -4470,13 +4470,13 @@
         <v>8.7421918242865937E-3</v>
       </c>
       <c r="J114" s="2">
-        <v>1.435057468892572E-2</v>
+        <v>1.4466337307494481E-2</v>
       </c>
       <c r="K114" s="2">
         <v>7.2663305193933041E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>42916</v>
       </c>
@@ -4505,13 +4505,13 @@
         <v>-1.197183756463915E-3</v>
       </c>
       <c r="J115" s="2">
-        <v>6.3999239363830181E-3</v>
+        <v>6.4659215292236002E-3</v>
       </c>
       <c r="K115" s="2">
-        <v>4.1426181352242821E-4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.1426181352242832E-4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>42947</v>
       </c>
@@ -4540,13 +4540,13 @@
         <v>3.462301040589377E-3</v>
       </c>
       <c r="J116" s="2">
-        <v>1.9606324749366591E-2</v>
+        <v>1.920780951596978E-2</v>
       </c>
       <c r="K116" s="2">
         <v>-2.501449465013861E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>42978</v>
       </c>
@@ -4575,13 +4575,13 @@
         <v>1.3932807960472581E-3</v>
       </c>
       <c r="J117" s="2">
-        <v>2.7501564804740821E-3</v>
+        <v>2.6205448099233491E-3</v>
       </c>
       <c r="K117" s="2">
         <v>-8.1356248591845336E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>43008</v>
       </c>
@@ -4610,13 +4610,13 @@
         <v>3.515512070982552E-3</v>
       </c>
       <c r="J118" s="2">
-        <v>1.9926850940756542E-2</v>
+        <v>1.9634716159554959E-2</v>
       </c>
       <c r="K118" s="2">
         <v>-1.833707549696115E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>43039</v>
       </c>
@@ -4645,13 +4645,13 @@
         <v>5.4642170802854158E-3</v>
       </c>
       <c r="J119" s="2">
-        <v>2.390427962271921E-2</v>
+        <v>2.4141284253566032E-2</v>
       </c>
       <c r="K119" s="2">
         <v>1.4876598367000559E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>43069</v>
       </c>
@@ -4680,13 +4680,13 @@
         <v>-2.466848165096857E-3</v>
       </c>
       <c r="J120" s="2">
-        <v>3.0169581051901009E-2</v>
+        <v>2.9961178122577009E-2</v>
       </c>
       <c r="K120" s="2">
         <v>-1.308129156372225E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>43100</v>
       </c>
@@ -4715,13 +4715,13 @@
         <v>5.7396833021414956E-3</v>
       </c>
       <c r="J121" s="2">
-        <v>9.5396294918244588E-3</v>
+        <v>8.8816674318507368E-3</v>
       </c>
       <c r="K121" s="2">
-        <v>-4.1299772379888968E-3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-4.1299772379888976E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>43131</v>
       </c>
@@ -4750,13 +4750,13 @@
         <v>-4.2338727731142563E-3</v>
       </c>
       <c r="J122" s="2">
-        <v>5.85360642712483E-2</v>
+        <v>5.9070300305540897E-2</v>
       </c>
       <c r="K122" s="2">
         <v>3.3533584921750519E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>43159</v>
       </c>
@@ -4785,13 +4785,13 @@
         <v>-2.654289277610656E-3</v>
       </c>
       <c r="J123" s="2">
-        <v>-3.6864248392521969E-2</v>
+        <v>-3.686725452392553E-2</v>
       </c>
       <c r="K123" s="2">
-        <v>-1.8869255579274671E-5</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-1.8869255579274461E-5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>43190</v>
       </c>
@@ -4820,13 +4820,13 @@
         <v>-1.194371544304251E-3</v>
       </c>
       <c r="J124" s="2">
-        <v>-2.4622017536702751E-2</v>
+        <v>-2.4292317087836031E-2</v>
       </c>
       <c r="K124" s="2">
         <v>2.0695043559634321E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>43220</v>
       </c>
@@ -4855,13 +4855,13 @@
         <v>4.317617068899215E-4</v>
       </c>
       <c r="J125" s="2">
-        <v>2.6474093753021369E-3</v>
+        <v>2.151709071049866E-3</v>
       </c>
       <c r="K125" s="2">
-        <v>-3.1114726789988772E-3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.1114726789988759E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>43251</v>
       </c>
@@ -4890,13 +4890,13 @@
         <v>-1.3508703594942611E-3</v>
       </c>
       <c r="J126" s="2">
-        <v>2.366331596802615E-2</v>
+        <v>2.3488929548610399E-2</v>
       </c>
       <c r="K126" s="2">
         <v>-1.0946101403326719E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>43281</v>
       </c>
@@ -4925,13 +4925,13 @@
         <v>7.1316917299836906E-3</v>
       </c>
       <c r="J127" s="2">
-        <v>6.8564417357696427E-3</v>
+        <v>7.1487012394753366E-3</v>
       </c>
       <c r="K127" s="2">
         <v>1.834490423260355E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>43312</v>
       </c>
@@ -4960,13 +4960,13 @@
         <v>2.2879875734213911E-3</v>
       </c>
       <c r="J128" s="2">
-        <v>3.6825517396533683E-2</v>
+        <v>3.6663794641855041E-2</v>
       </c>
       <c r="K128" s="2">
-        <v>-1.0151212909058631E-3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-1.015121290905862E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>43343</v>
       </c>
@@ -4995,13 +4995,13 @@
         <v>1.919811401395588E-3</v>
       </c>
       <c r="J129" s="2">
-        <v>3.2679876867036252E-2</v>
+        <v>3.2719282487058937E-2</v>
       </c>
       <c r="K129" s="2">
         <v>2.4734604568086047E-4</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>43373</v>
       </c>
@@ -5030,13 +5030,13 @@
         <v>1.1780380331690619E-2</v>
       </c>
       <c r="J130" s="2">
-        <v>5.5515822590650101E-3</v>
+        <v>5.4931279919082331E-3</v>
       </c>
       <c r="K130" s="2">
-        <v>-3.6691293846101268E-4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.6691293846101289E-4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>43404</v>
       </c>
@@ -5065,13 +5065,13 @@
         <v>2.7428663889505259E-3</v>
       </c>
       <c r="J131" s="2">
-        <v>-6.5278625919716282E-2</v>
+        <v>-6.3998806739625561E-2</v>
       </c>
       <c r="K131" s="2">
         <v>8.0333265458002543E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>43434</v>
       </c>
@@ -5100,13 +5100,13 @@
         <v>6.6789812456414799E-3</v>
       </c>
       <c r="J132" s="2">
-        <v>2.0293018293863721E-2</v>
+        <v>2.0257414289975281E-2</v>
       </c>
       <c r="K132" s="2">
-        <v>-2.2348359363818509E-4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-2.2348359363818479E-4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>43465</v>
       </c>
@@ -5135,13 +5135,13 @@
         <v>-5.9638096672464773E-3</v>
       </c>
       <c r="J133" s="2">
-        <v>-9.0948281434138953E-2</v>
+        <v>-9.1222189284501071E-2</v>
       </c>
       <c r="K133" s="2">
         <v>-1.719298506888352E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>43496</v>
       </c>
@@ -5170,13 +5170,13 @@
         <v>-1.864903598181067E-3</v>
       </c>
       <c r="J134" s="2">
-        <v>7.8226984040746128E-2</v>
+        <v>7.7431578573399218E-2</v>
       </c>
       <c r="K134" s="2">
         <v>-4.992698933500692E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>43524</v>
       </c>
@@ -5205,13 +5205,13 @@
         <v>4.0653482303681489E-3</v>
       </c>
       <c r="J135" s="2">
-        <v>3.1686916413699528E-2</v>
+        <v>3.151143831531085E-2</v>
       </c>
       <c r="K135" s="2">
         <v>-1.101462525270439E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>43555</v>
       </c>
@@ -5240,13 +5240,13 @@
         <v>-2.7228366209964602E-3</v>
       </c>
       <c r="J136" s="2">
-        <v>1.8640853708045361E-2</v>
+        <v>1.8311262936729411E-2</v>
       </c>
       <c r="K136" s="2">
         <v>-2.068815918414024E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>43585</v>
       </c>
@@ -5275,13 +5275,13 @@
         <v>7.0828676824820757E-3</v>
       </c>
       <c r="J137" s="2">
-        <v>3.9909222564152677E-2</v>
+        <v>3.9667386943062592E-2</v>
       </c>
       <c r="K137" s="2">
         <v>-1.5179835908423411E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>43616</v>
       </c>
@@ -5310,13 +5310,13 @@
         <v>-1.08397443944005E-2</v>
       </c>
       <c r="J138" s="2">
-        <v>-6.3651589399977171E-2</v>
+        <v>-6.3694691956034333E-2</v>
       </c>
       <c r="K138" s="2">
-        <v>-2.7055142878950299E-4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-2.705514287895032E-4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>43646</v>
       </c>
@@ -5345,13 +5345,13 @@
         <v>7.7680358953529536E-3</v>
       </c>
       <c r="J139" s="2">
-        <v>7.016657437290616E-2</v>
+        <v>7.0037598291801381E-2</v>
       </c>
       <c r="K139" s="2">
-        <v>-8.0957293985768793E-4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-8.0957293985768814E-4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>43677</v>
       </c>
@@ -5380,13 +5380,13 @@
         <v>3.9355856539855516E-3</v>
       </c>
       <c r="J140" s="2">
-        <v>1.366084374341635E-2</v>
+        <v>1.336441462730144E-2</v>
       </c>
       <c r="K140" s="2">
         <v>-1.860662759613621E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>43708</v>
       </c>
@@ -5415,13 +5415,13 @@
         <v>-9.2579167563885973E-3</v>
       </c>
       <c r="J141" s="2">
-        <v>-1.4329902861036369E-2</v>
+        <v>-1.370053925269658E-2</v>
       </c>
       <c r="K141" s="2">
         <v>3.9504669569636539E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>43738</v>
       </c>
@@ -5450,13 +5450,13 @@
         <v>1.3945968547556699E-2</v>
       </c>
       <c r="J142" s="2">
-        <v>1.8286647068731392E-2</v>
+        <v>1.8110103128212259E-2</v>
       </c>
       <c r="K142" s="2">
         <v>-1.1081527343354629E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>43769</v>
       </c>
@@ -5485,13 +5485,13 @@
         <v>-2.904878704725345E-3</v>
       </c>
       <c r="J143" s="2">
-        <v>1.923816989088728E-2</v>
+        <v>1.8229147476358409E-2</v>
       </c>
       <c r="K143" s="2">
-        <v>-6.3335560788889602E-3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-6.3335560788889576E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>43799</v>
       </c>
@@ -5520,13 +5520,13 @@
         <v>2.927030703338484E-3</v>
       </c>
       <c r="J144" s="2">
-        <v>3.6690259615353008E-2</v>
+        <v>3.6853348377387123E-2</v>
       </c>
       <c r="K144" s="2">
         <v>1.023695613998849E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>43830</v>
       </c>
@@ -5555,13 +5555,13 @@
         <v>3.0176346736779051E-3</v>
       </c>
       <c r="J145" s="2">
-        <v>2.7976912176471219E-2</v>
+        <v>2.7058107548461031E-2</v>
       </c>
       <c r="K145" s="2">
         <v>-5.7672659727408676E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>43861</v>
       </c>
@@ -5590,13 +5590,13 @@
         <v>1.72636644008155E-3</v>
       </c>
       <c r="J146" s="2">
-        <v>4.2619507554394283E-4</v>
+        <v>7.6717332946926362E-4</v>
       </c>
       <c r="K146" s="2">
         <v>2.1402942707927832E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>43890</v>
       </c>
@@ -5625,13 +5625,13 @@
         <v>-1.9519811696924062E-2</v>
       </c>
       <c r="J147" s="2">
-        <v>-7.4971513074322649E-2</v>
+        <v>-7.1909976656898258E-2</v>
       </c>
       <c r="K147" s="2">
         <v>1.9217028589371511E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>43921</v>
       </c>
@@ -5660,13 +5660,13 @@
         <v>9.7783028682561668E-2</v>
       </c>
       <c r="J148" s="2">
-        <v>-5.3578832404057468E-2</v>
+        <v>-2.443968693881143E-2</v>
       </c>
       <c r="K148" s="2">
         <v>0.1829041746126214</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>43951</v>
       </c>
@@ -5695,13 +5695,13 @@
         <v>-3.3981213000015991E-3</v>
       </c>
       <c r="J149" s="2">
-        <v>0.1294083608113317</v>
+        <v>0.129914419841552</v>
       </c>
       <c r="K149" s="2">
         <v>3.1764936050750919E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>43982</v>
       </c>
@@ -5730,13 +5730,13 @@
         <v>-2.2750897116867951E-3</v>
       </c>
       <c r="J150" s="2">
-        <v>4.646691595416353E-2</v>
+        <v>4.5983146287727657E-2</v>
       </c>
       <c r="K150" s="2">
         <v>-3.0365849831666932E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>44012</v>
       </c>
@@ -5765,13 +5765,13 @@
         <v>-7.2633546834797811E-3</v>
       </c>
       <c r="J151" s="2">
-        <v>1.903031519830085E-2</v>
+        <v>1.8673263987471551E-2</v>
       </c>
       <c r="K151" s="2">
         <v>-2.2411829848977389E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>44043</v>
       </c>
@@ -5800,13 +5800,13 @@
         <v>2.7126912308021332E-3</v>
       </c>
       <c r="J152" s="2">
-        <v>5.7483947874128707E-2</v>
+        <v>5.7941826014742841E-2</v>
       </c>
       <c r="K152" s="2">
-        <v>2.874065867239429E-3</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.8740658672394299E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>44074</v>
       </c>
@@ -5835,13 +5835,13 @@
         <v>1.1897102877061E-2</v>
       </c>
       <c r="J153" s="2">
-        <v>7.6346602278110409E-2</v>
+        <v>7.8207429181133561E-2</v>
       </c>
       <c r="K153" s="2">
-        <v>1.1680267329745289E-2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.16802673297453E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>44104</v>
       </c>
@@ -5870,13 +5870,13 @@
         <v>-2.6088229928169018E-2</v>
       </c>
       <c r="J154" s="2">
-        <v>-4.5157188917358981E-2</v>
+        <v>-4.814075400819344E-2</v>
       </c>
       <c r="K154" s="2">
         <v>-1.8727608570160939E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>44135</v>
       </c>
@@ -5905,13 +5905,13 @@
         <v>6.6492114820448931E-3</v>
       </c>
       <c r="J155" s="2">
-        <v>-2.6354835379044369E-2</v>
+        <v>-2.6255273665726719E-2</v>
       </c>
       <c r="K155" s="2">
-        <v>6.2494121590154703E-4</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.2494121590154692E-4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>44165</v>
       </c>
@@ -5940,13 +5940,13 @@
         <v>5.250768674645032E-5</v>
       </c>
       <c r="J156" s="2">
-        <v>0.1067996382572996</v>
+        <v>0.10568956160918599</v>
       </c>
       <c r="K156" s="2">
         <v>-6.9678657296975838E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>44196</v>
       </c>
@@ -5975,13 +5975,13 @@
         <v>1.099009619429667E-2</v>
       </c>
       <c r="J157" s="2">
-        <v>3.9040077551498333E-2</v>
+        <v>3.9286703257411217E-2</v>
       </c>
       <c r="K157" s="2">
         <v>1.5480505848070091E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>44227</v>
       </c>
@@ -6010,13 +6010,13 @@
         <v>9.7262976414237874E-3</v>
       </c>
       <c r="J158" s="2">
-        <v>-6.86380289439204E-3</v>
+        <v>-5.5171801376594897E-3</v>
       </c>
       <c r="K158" s="2">
         <v>8.452647457644338E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>44255</v>
       </c>
@@ -6045,13 +6045,13 @@
         <v>4.8994026137382908E-3</v>
       </c>
       <c r="J159" s="2">
-        <v>3.0276387396719631E-2</v>
+        <v>3.1402010132921487E-2</v>
       </c>
       <c r="K159" s="2">
         <v>7.0654473287747738E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>44286</v>
       </c>
@@ -6080,13 +6080,13 @@
         <v>2.8369345032142612E-3</v>
       </c>
       <c r="J160" s="2">
-        <v>4.3123914532099523E-2</v>
+        <v>4.2844015877999672E-2</v>
       </c>
       <c r="K160" s="2">
         <v>-1.756902321119116E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>44316</v>
       </c>
@@ -6115,13 +6115,13 @@
         <v>-4.0861571348999367E-3</v>
       </c>
       <c r="J161" s="2">
-        <v>5.1934296820780101E-2</v>
+        <v>5.133658471139009E-2</v>
       </c>
       <c r="K161" s="2">
         <v>-3.7517929327866031E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>44347</v>
       </c>
@@ -6150,13 +6150,13 @@
         <v>-6.7689182858616586E-3</v>
       </c>
       <c r="J162" s="2">
-        <v>5.5681675708055224E-3</v>
+        <v>4.9781066242538174E-3</v>
       </c>
       <c r="K162" s="2">
         <v>-3.703767172201488E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>44377</v>
       </c>
@@ -6185,13 +6185,13 @@
         <v>8.7678942765357683E-3</v>
       </c>
       <c r="J163" s="2">
-        <v>2.2305232125971072E-2</v>
+        <v>2.1872073342140461E-2</v>
       </c>
       <c r="K163" s="2">
         <v>-2.7189043661982899E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>44408</v>
       </c>
@@ -6220,13 +6220,13 @@
         <v>-1.23674868585131E-2</v>
       </c>
       <c r="J164" s="2">
-        <v>2.1366246547384331E-2</v>
+        <v>2.0370963715602819E-2</v>
       </c>
       <c r="K164" s="2">
-        <v>-6.2473137748747416E-3</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-6.2473137748747434E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>44439</v>
       </c>
@@ -6255,13 +6255,13 @@
         <v>-4.7468970458997674E-3</v>
       </c>
       <c r="J165" s="2">
-        <v>2.9747953188646141E-2</v>
+        <v>2.947392066706761E-2</v>
       </c>
       <c r="K165" s="2">
         <v>-1.7200810585236989E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>44469</v>
       </c>
@@ -6290,13 +6290,13 @@
         <v>6.6972309828241539E-3</v>
       </c>
       <c r="J166" s="2">
-        <v>-4.6815087743838753E-2</v>
+        <v>-4.6942291505035393E-2</v>
       </c>
       <c r="K166" s="2">
         <v>-7.9844822412661028E-4</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>44500</v>
       </c>
@@ -6325,13 +6325,13 @@
         <v>1.672229346085464E-3</v>
       </c>
       <c r="J167" s="2">
-        <v>7.1903372095515755E-2</v>
+        <v>7.2670686407471957E-2</v>
       </c>
       <c r="K167" s="2">
-        <v>4.8163729119712617E-3</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.8163729119712626E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>44530</v>
       </c>
@@ -6360,13 +6360,13 @@
         <v>3.1213066951772512E-3</v>
       </c>
       <c r="J168" s="2">
-        <v>-5.1091858733504931E-3</v>
+        <v>-4.3509636424942568E-3</v>
       </c>
       <c r="K168" s="2">
         <v>4.7593026182976101E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>44561</v>
       </c>
@@ -6395,13 +6395,13 @@
         <v>-1.7462424820528451E-2</v>
       </c>
       <c r="J169" s="2">
-        <v>4.0742580139748671E-2</v>
+        <v>3.9045285338741402E-2</v>
       </c>
       <c r="K169" s="2">
         <v>-1.0653788904784189E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>44592</v>
       </c>
@@ -6430,13 +6430,13 @@
         <v>-3.1890271885302413E-2</v>
       </c>
       <c r="J170" s="2">
-        <v>-5.2992653724795162E-2</v>
+        <v>-5.3511661983251531E-2</v>
       </c>
       <c r="K170" s="2">
         <v>-3.2577749146184588E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>44620</v>
       </c>
@@ -6465,13 +6465,13 @@
         <v>-6.0898972370416733E-4</v>
       </c>
       <c r="J171" s="2">
-        <v>-2.782135698898397E-2</v>
+        <v>-2.6937985623444769E-2</v>
       </c>
       <c r="K171" s="2">
         <v>5.5448541098461358E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>44651</v>
       </c>
@@ -6500,19 +6500,264 @@
         <v>2.6180172166168749E-3</v>
       </c>
       <c r="J172" s="2">
-        <v>3.8611639753957483E-2</v>
+        <v>3.9229172417169673E-2</v>
       </c>
       <c r="K172" s="2">
         <v>3.8762050244703942E-3</v>
       </c>
     </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A173" s="3">
+        <v>44681</v>
+      </c>
+      <c r="B173" s="2">
+        <v>-8.7201844689124286E-2</v>
+      </c>
+      <c r="C173" s="2">
+        <v>-2.0343792770055599E-2</v>
+      </c>
+      <c r="D173" s="2">
+        <v>3.604596856313869E-3</v>
+      </c>
+      <c r="E173" s="2">
+        <v>2.9718382942591551E-2</v>
+      </c>
+      <c r="F173" s="2">
+        <v>1.7260536242822101E-3</v>
+      </c>
+      <c r="G173" s="2">
+        <v>1.3112527426601069E-2</v>
+      </c>
+      <c r="H173" s="2">
+        <v>7.0947547462596461E-3</v>
+      </c>
+      <c r="I173" s="2">
+        <v>3.28176911031588E-3</v>
+      </c>
+      <c r="J173" s="2">
+        <v>-8.438731343156658E-2</v>
+      </c>
+      <c r="K173" s="2">
+        <v>5.196057706260364E-3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A174" s="3">
+        <v>44712</v>
+      </c>
+      <c r="B174" s="2">
+        <v>1.8346151108581401E-3</v>
+      </c>
+      <c r="C174" s="2">
+        <v>-1.4830233305306639E-2</v>
+      </c>
+      <c r="D174" s="2">
+        <v>-1.612962287670738E-2</v>
+      </c>
+      <c r="E174" s="2">
+        <v>5.0964313527877003E-3</v>
+      </c>
+      <c r="F174" s="2">
+        <v>-4.0537692093064938E-2</v>
+      </c>
+      <c r="G174" s="2">
+        <v>4.3228656388043518E-3</v>
+      </c>
+      <c r="H174" s="2">
+        <v>3.331670277789045E-2</v>
+      </c>
+      <c r="I174" s="2">
+        <v>-4.4507081742510609E-3</v>
+      </c>
+      <c r="J174" s="2">
+        <v>-3.351400679345376E-3</v>
+      </c>
+      <c r="K174" s="2">
+        <v>-9.5741829972987996E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A175" s="3">
+        <v>44742</v>
+      </c>
+      <c r="B175" s="2">
+        <v>-8.254376821069076E-2</v>
+      </c>
+      <c r="C175" s="2">
+        <v>-3.6804526798941077E-2</v>
+      </c>
+      <c r="D175" s="2">
+        <v>-6.180626902126507E-3</v>
+      </c>
+      <c r="E175" s="2">
+        <v>2.9489180843426999E-2</v>
+      </c>
+      <c r="F175" s="2">
+        <v>1.6609288778682361E-2</v>
+      </c>
+      <c r="G175" s="2">
+        <v>-1.0944626522107479E-2</v>
+      </c>
+      <c r="H175" s="2">
+        <v>-2.5056335894324658E-2</v>
+      </c>
+      <c r="I175" s="2">
+        <v>-2.400110169929959E-3</v>
+      </c>
+      <c r="J175" s="2">
+        <v>-8.4047156666533132E-2</v>
+      </c>
+      <c r="K175" s="2">
+        <v>-2.775486380016685E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A176" s="3">
+        <v>44773</v>
+      </c>
+      <c r="B176" s="2">
+        <v>9.2204461388357473E-2</v>
+      </c>
+      <c r="C176" s="2">
+        <v>1.327123640954442E-2</v>
+      </c>
+      <c r="D176" s="2">
+        <v>-5.2601848788800254E-3</v>
+      </c>
+      <c r="E176" s="2">
+        <v>-2.2822610100831201E-2</v>
+      </c>
+      <c r="F176" s="2">
+        <v>-2.3513183755391829E-2</v>
+      </c>
+      <c r="G176" s="2">
+        <v>-1.098787008357704E-2</v>
+      </c>
+      <c r="H176" s="2">
+        <v>-9.8113366034290328E-3</v>
+      </c>
+      <c r="I176" s="2">
+        <v>5.5413215244666247E-3</v>
+      </c>
+      <c r="J176" s="2">
+        <v>8.8242863783753622E-2</v>
+      </c>
+      <c r="K176" s="2">
+        <v>-7.3137186546532807E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A177" s="3">
+        <v>44804</v>
+      </c>
+      <c r="B177" s="2">
+        <v>-4.0781924345117633E-2</v>
+      </c>
+      <c r="C177" s="2">
+        <v>-1.7873202637612721E-2</v>
+      </c>
+      <c r="D177" s="2">
+        <v>-6.7296123335447433E-4</v>
+      </c>
+      <c r="E177" s="2">
+        <v>1.094158822929758E-2</v>
+      </c>
+      <c r="F177" s="2">
+        <v>2.274759671561296E-2</v>
+      </c>
+      <c r="G177" s="2">
+        <v>-7.6719854433480172E-3</v>
+      </c>
+      <c r="H177" s="2">
+        <v>9.3444301018108522E-3</v>
+      </c>
+      <c r="I177" s="2">
+        <v>8.0094517179815309E-3</v>
+      </c>
+      <c r="J177" s="2">
+        <v>-3.9311228131310043E-2</v>
+      </c>
+      <c r="K177" s="2">
+        <v>2.7151314716447618E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A178" s="3">
+        <v>44834</v>
+      </c>
+      <c r="B178" s="2">
+        <v>-9.2098601263658209E-2</v>
+      </c>
+      <c r="C178" s="2">
+        <v>-3.1695302348644587E-2</v>
+      </c>
+      <c r="D178" s="2">
+        <v>1.696093882445959E-3</v>
+      </c>
+      <c r="E178" s="2">
+        <v>3.1942903879981673E-2</v>
+      </c>
+      <c r="F178" s="2">
+        <v>5.3332722001232923E-2</v>
+      </c>
+      <c r="G178" s="2">
+        <v>-1.1989244942036681E-3</v>
+      </c>
+      <c r="H178" s="2">
+        <v>1.0964386230749581E-3</v>
+      </c>
+      <c r="I178" s="2">
+        <v>2.9521574700462241E-3</v>
+      </c>
+      <c r="J178" s="2">
+        <v>-8.7287952637221625E-2</v>
+      </c>
+      <c r="K178" s="2">
+        <v>8.8811974641905753E-3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A179" s="3">
+        <v>44865</v>
+      </c>
+      <c r="B179" s="2">
+        <v>8.0961375978148009E-2</v>
+      </c>
+      <c r="C179" s="2">
+        <v>1.0058685007288791E-2</v>
+      </c>
+      <c r="D179" s="2">
+        <v>-6.6937509059638023E-3</v>
+      </c>
+      <c r="E179" s="2">
+        <v>-2.159515330495965E-2</v>
+      </c>
+      <c r="F179" s="2">
+        <v>-1.6345565174648281E-2</v>
+      </c>
+      <c r="G179" s="2">
+        <v>-4.1747941288096113E-3</v>
+      </c>
+      <c r="H179" s="2">
+        <v>-3.5372226925148957E-2</v>
+      </c>
+      <c r="I179" s="2">
+        <v>-3.848582855877625E-3</v>
+      </c>
+      <c r="J179" s="2">
+        <v>7.6535071326418971E-2</v>
+      </c>
+      <c r="K179" s="2">
+        <v>-8.1716393570382111E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A172">
+  <conditionalFormatting sqref="A1:A179">
     <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:K172">
+  <conditionalFormatting sqref="B2:K179">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update equity hedge data 9/29/23
</commit_message>
<xml_diff>
--- a/data/time_series/equity_hedge_data.xlsx
+++ b/data/time_series/equity_hedge_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloomberg\Documents\GitHub\UPS_MV\data\time_series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8380189-DD26-4B6E-8373-46BBA2910D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Historical Returns" sheetId="3" r:id="rId1"/>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
@@ -154,7 +155,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -479,19 +510,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALM169"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:ALM170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169:M170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1001" width="21.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1001" width="21.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>40086</v>
       </c>
@@ -573,7 +604,7 @@
         <v>1.4960839298960491E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>40117</v>
       </c>
@@ -614,7 +645,7 @@
         <v>8.5898158422219976E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>40147</v>
       </c>
@@ -655,7 +686,7 @@
         <v>1.5716762227836461E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>40178</v>
       </c>
@@ -696,7 +727,7 @@
         <v>5.720081133514493E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>40209</v>
       </c>
@@ -737,7 +768,7 @@
         <v>4.9845162439586888E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>40237</v>
       </c>
@@ -778,7 +809,7 @@
         <v>-7.5188107119393043E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>40268</v>
       </c>
@@ -819,7 +850,7 @@
         <v>8.9100415074582005E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>40298</v>
       </c>
@@ -860,7 +891,7 @@
         <v>7.7852467079566803E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>40329</v>
       </c>
@@ -901,7 +932,7 @@
         <v>-2.7403044899580679E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>40359</v>
       </c>
@@ -942,7 +973,7 @@
         <v>1.1444728351439519E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>40390</v>
       </c>
@@ -983,7 +1014,7 @@
         <v>-4.6795666813305358E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>40421</v>
       </c>
@@ -1024,7 +1055,7 @@
         <v>1.170321011363336E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>40451</v>
       </c>
@@ -1065,7 +1096,7 @@
         <v>6.9581318404216561E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>40482</v>
       </c>
@@ -1106,7 +1137,7 @@
         <v>-4.4348550807638814E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>40512</v>
       </c>
@@ -1147,7 +1178,7 @@
         <v>7.6120853520938794E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>40543</v>
       </c>
@@ -1188,7 +1219,7 @@
         <v>5.9248463917495027E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>40574</v>
       </c>
@@ -1229,7 +1260,7 @@
         <v>8.1889197257202714E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>40602</v>
       </c>
@@ -1270,7 +1301,7 @@
         <v>2.8071421376937622E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>40633</v>
       </c>
@@ -1311,7 +1342,7 @@
         <v>2.0257567115102219E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>40663</v>
       </c>
@@ -1352,7 +1383,7 @@
         <v>2.4310354786327118E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>40694</v>
       </c>
@@ -1393,7 +1424,7 @@
         <v>2.3099732794387099E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>40724</v>
       </c>
@@ -1434,7 +1465,7 @@
         <v>8.7471352928429451E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>40755</v>
       </c>
@@ -1475,7 +1506,7 @@
         <v>4.7567340953178364E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>40786</v>
       </c>
@@ -1516,7 +1547,7 @@
         <v>2.003093517453107E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>40816</v>
       </c>
@@ -1557,7 +1588,7 @@
         <v>1.2960977414519339E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>40847</v>
       </c>
@@ -1598,7 +1629,7 @@
         <v>-4.0412481453216929E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>40877</v>
       </c>
@@ -1639,7 +1670,7 @@
         <v>8.8433159826027917E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>40908</v>
       </c>
@@ -1680,7 +1711,7 @@
         <v>3.5015888603789712E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>40939</v>
       </c>
@@ -1721,7 +1752,7 @@
         <v>-2.6971758070874091E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>40968</v>
       </c>
@@ -1762,7 +1793,7 @@
         <v>5.6698230561319143E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>40999</v>
       </c>
@@ -1803,7 +1834,7 @@
         <v>-2.8371420206049149E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>41029</v>
       </c>
@@ -1844,7 +1875,7 @@
         <v>-1.378009030609468E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>41060</v>
       </c>
@@ -1885,7 +1916,7 @@
         <v>4.5540985898174799E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>41090</v>
       </c>
@@ -1926,7 +1957,7 @@
         <v>1.6071933956403671E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>41121</v>
       </c>
@@ -1967,7 +1998,7 @@
         <v>-3.518820966340307E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>41152</v>
       </c>
@@ -2008,7 +2039,7 @@
         <v>3.5436568351997488E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>41182</v>
       </c>
@@ -2049,7 +2080,7 @@
         <v>-5.4147879048632918E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>41213</v>
       </c>
@@ -2090,7 +2121,7 @@
         <v>9.3041372562262833E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>41243</v>
       </c>
@@ -2131,7 +2162,7 @@
         <v>4.1008688945848122E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41274</v>
       </c>
@@ -2172,7 +2203,7 @@
         <v>5.4790889883789013E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41305</v>
       </c>
@@ -2213,7 +2244,7 @@
         <v>1.3260819769358139E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>41333</v>
       </c>
@@ -2254,7 +2285,7 @@
         <v>2.5580118994295931E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>41364</v>
       </c>
@@ -2295,7 +2326,7 @@
         <v>4.9676251080680255E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>41394</v>
       </c>
@@ -2336,7 +2367,7 @@
         <v>-4.7231586306693231E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>41425</v>
       </c>
@@ -2377,7 +2408,7 @@
         <v>2.1892887610491041E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>41455</v>
       </c>
@@ -2418,7 +2449,7 @@
         <v>2.316827316875348E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>41486</v>
       </c>
@@ -2459,7 +2490,7 @@
         <v>3.9205369250465008E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>41517</v>
       </c>
@@ -2500,7 +2531,7 @@
         <v>4.163733421821642E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>41547</v>
       </c>
@@ -2541,7 +2572,7 @@
         <v>-1.7308398012315319E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>41578</v>
       </c>
@@ -2582,7 +2613,7 @@
         <v>9.6249457802273096E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>41608</v>
       </c>
@@ -2623,7 +2654,7 @@
         <v>1.3278603581516281E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>41639</v>
       </c>
@@ -2664,7 +2695,7 @@
         <v>2.584178411290564E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>41670</v>
       </c>
@@ -2705,7 +2736,7 @@
         <v>-1.135869620985411E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>41698</v>
       </c>
@@ -2746,7 +2777,7 @@
         <v>-5.274519712912568E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>41729</v>
       </c>
@@ -2787,7 +2818,7 @@
         <v>1.0548407872170149E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>41759</v>
       </c>
@@ -2828,7 +2859,7 @@
         <v>7.5631536878732181E-5</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>41790</v>
       </c>
@@ -2869,7 +2900,7 @@
         <v>1.7265273583676991E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>41820</v>
       </c>
@@ -2910,7 +2941,7 @@
         <v>-9.1654664568851716E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>41851</v>
       </c>
@@ -2951,7 +2982,7 @@
         <v>3.1287434322478389E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>41882</v>
       </c>
@@ -2992,7 +3023,7 @@
         <v>2.628684671229716E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>41912</v>
       </c>
@@ -3033,7 +3064,7 @@
         <v>-7.0789447438400217E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>41943</v>
       </c>
@@ -3074,7 +3105,7 @@
         <v>4.1154433698597807E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>41973</v>
       </c>
@@ -3115,7 +3146,7 @@
         <v>1.727698339506918E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>42004</v>
       </c>
@@ -3156,7 +3187,7 @@
         <v>4.2032350787960804E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>42035</v>
       </c>
@@ -3197,7 +3228,7 @@
         <v>7.0341934730231426E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>42063</v>
       </c>
@@ -3238,7 +3269,7 @@
         <v>-3.4020933981551778E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>42094</v>
       </c>
@@ -3279,7 +3310,7 @@
         <v>2.102345486467132E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>42124</v>
       </c>
@@ -3320,7 +3351,7 @@
         <v>-1.6879291581832711E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>42155</v>
       </c>
@@ -3361,7 +3392,7 @@
         <v>-5.316805390114073E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>42185</v>
       </c>
@@ -3402,7 +3433,7 @@
         <v>2.0067464933851312E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>42216</v>
       </c>
@@ -3443,7 +3474,7 @@
         <v>4.2976958108435992E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>42247</v>
       </c>
@@ -3484,7 +3515,7 @@
         <v>8.9957609586586839E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>42277</v>
       </c>
@@ -3525,7 +3556,7 @@
         <v>2.6740076906067692E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>42308</v>
       </c>
@@ -3566,7 +3597,7 @@
         <v>-6.8388219488078807E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>42338</v>
       </c>
@@ -3607,7 +3638,7 @@
         <v>2.6162607802293191E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>42369</v>
       </c>
@@ -3648,7 +3679,7 @@
         <v>-2.0487381042651638E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>42400</v>
       </c>
@@ -3689,7 +3720,7 @@
         <v>7.6232839368307638E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>42429</v>
       </c>
@@ -3730,7 +3761,7 @@
         <v>4.2742596680992876E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>42460</v>
       </c>
@@ -3771,7 +3802,7 @@
         <v>-1.031645365033245E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>42490</v>
       </c>
@@ -3812,7 +3843,7 @@
         <v>-7.4352364122333046E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>42521</v>
       </c>
@@ -3853,7 +3884,7 @@
         <v>-1.3476761949897699E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>42551</v>
       </c>
@@ -3894,7 +3925,7 @@
         <v>5.1711890781862956E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>42582</v>
       </c>
@@ -3935,7 +3966,7 @@
         <v>-1.374675761171968E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>42613</v>
       </c>
@@ -3976,7 +4007,7 @@
         <v>3.490180937263871E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>42643</v>
       </c>
@@ -4017,7 +4048,7 @@
         <v>-1.7247001438739911E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>42674</v>
       </c>
@@ -4058,7 +4089,7 @@
         <v>-5.5001353414474115E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>42704</v>
       </c>
@@ -4099,7 +4130,7 @@
         <v>1.084823024870248E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>42735</v>
       </c>
@@ -4140,7 +4171,7 @@
         <v>1.8712457277628681E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>42766</v>
       </c>
@@ -4181,7 +4212,7 @@
         <v>-2.785744411213464E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>42794</v>
       </c>
@@ -4222,7 +4253,7 @@
         <v>2.566898308698331E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>42825</v>
       </c>
@@ -4263,7 +4294,7 @@
         <v>-3.2633923773821398E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>42855</v>
       </c>
@@ -4304,7 +4335,7 @@
         <v>-2.6328129581849719E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>42886</v>
       </c>
@@ -4345,7 +4376,7 @@
         <v>6.3346776271822221E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>42916</v>
       </c>
@@ -4386,7 +4417,7 @@
         <v>4.9335424480035793E-4</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>42947</v>
       </c>
@@ -4427,7 +4458,7 @@
         <v>-2.4038901120139152E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>42978</v>
       </c>
@@ -4468,7 +4499,7 @@
         <v>5.5318088627688631E-4</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>43008</v>
       </c>
@@ -4509,7 +4540,7 @@
         <v>-2.0886574879192378E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>43039</v>
       </c>
@@ -4550,7 +4581,7 @@
         <v>1.233494436020668E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>43069</v>
       </c>
@@ -4591,7 +4622,7 @@
         <v>-1.9905296835672211E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>43100</v>
       </c>
@@ -4632,7 +4663,7 @@
         <v>-4.216447904818268E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>43131</v>
       </c>
@@ -4673,7 +4704,7 @@
         <v>4.8907781513447043E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>43159</v>
       </c>
@@ -4714,7 +4745,7 @@
         <v>2.420803835524205E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>43190</v>
       </c>
@@ -4755,7 +4786,7 @@
         <v>2.5953686032865451E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>43220</v>
       </c>
@@ -4796,7 +4827,7 @@
         <v>-1.524008248151264E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>43251</v>
       </c>
@@ -4837,7 +4868,7 @@
         <v>-1.244127562954743E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>43281</v>
       </c>
@@ -4878,7 +4909,7 @@
         <v>1.9486079745118731E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>43312</v>
       </c>
@@ -4919,7 +4950,7 @@
         <v>-1.1556389345171579E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>43343</v>
       </c>
@@ -4960,7 +4991,7 @@
         <v>-4.4645788123386302E-7</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>43373</v>
       </c>
@@ -5001,7 +5032,7 @@
         <v>6.6085975750621105E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>43404</v>
       </c>
@@ -5042,7 +5073,7 @@
         <v>9.1372932795353683E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>43434</v>
       </c>
@@ -5083,7 +5114,7 @@
         <v>-1.061624715126852E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>43465</v>
       </c>
@@ -5124,7 +5155,7 @@
         <v>2.0128121019145169E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>43496</v>
       </c>
@@ -5165,7 +5196,7 @@
         <v>-3.7991759749694712E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>43524</v>
       </c>
@@ -5206,7 +5237,7 @@
         <v>-1.702753223627037E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>43555</v>
       </c>
@@ -5247,7 +5278,7 @@
         <v>-3.4769092556259429E-4</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>43585</v>
       </c>
@@ -5288,7 +5319,7 @@
         <v>-3.186142788395096E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>43616</v>
       </c>
@@ -5329,7 +5360,7 @@
         <v>3.0836483080191861E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>43646</v>
       </c>
@@ -5370,7 +5401,7 @@
         <v>-5.4917182997343459E-4</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>43677</v>
       </c>
@@ -5411,7 +5442,7 @@
         <v>-1.4977028405834111E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>43708</v>
       </c>
@@ -5452,7 +5483,7 @@
         <v>6.0880186730718688E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>43738</v>
       </c>
@@ -5493,7 +5524,7 @@
         <v>-1.966153270708885E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>43769</v>
       </c>
@@ -5534,7 +5565,7 @@
         <v>-5.0515475376806552E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>43799</v>
       </c>
@@ -5575,7 +5606,7 @@
         <v>4.9801416520831097E-4</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>43830</v>
       </c>
@@ -5616,7 +5647,7 @@
         <v>-4.4505950004874286E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>43861</v>
       </c>
@@ -5657,7 +5688,7 @@
         <v>2.5191611388298949E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>43890</v>
       </c>
@@ -5698,7 +5729,7 @@
         <v>1.45690092292672E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>43921</v>
       </c>
@@ -5739,7 +5770,7 @@
         <v>0.146876809973289</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>43951</v>
       </c>
@@ -5780,7 +5811,7 @@
         <v>2.862753617083822E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>43982</v>
       </c>
@@ -5821,7 +5852,7 @@
         <v>-1.6044363867557621E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>44012</v>
       </c>
@@ -5862,7 +5893,7 @@
         <v>-4.9612167980539369E-5</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>44043</v>
       </c>
@@ -5903,7 +5934,7 @@
         <v>2.7165083494641801E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>44074</v>
       </c>
@@ -5944,7 +5975,7 @@
         <v>7.3623377559711998E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>44104</v>
       </c>
@@ -5985,7 +6016,7 @@
         <v>-1.1997863583501651E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>44135</v>
       </c>
@@ -6026,7 +6057,7 @@
         <v>8.3442363645388074E-4</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>44165</v>
       </c>
@@ -6067,7 +6098,7 @@
         <v>-6.9997570862173376E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>44196</v>
       </c>
@@ -6108,7 +6139,7 @@
         <v>3.404369824934131E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>44227</v>
       </c>
@@ -6149,7 +6180,7 @@
         <v>9.2487050705139136E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>44255</v>
       </c>
@@ -6190,7 +6221,7 @@
         <v>7.2496200339918927E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>44286</v>
       </c>
@@ -6231,7 +6262,7 @@
         <v>7.2634395220755831E-4</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>44316</v>
       </c>
@@ -6272,7 +6303,7 @@
         <v>-2.95864280830165E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>44347</v>
       </c>
@@ -6313,7 +6344,7 @@
         <v>-3.2313837336500392E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>44377</v>
       </c>
@@ -6354,7 +6385,7 @@
         <v>-2.8683255675787168E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>44408</v>
       </c>
@@ -6395,7 +6426,7 @@
         <v>-3.7643833782831791E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>44439</v>
       </c>
@@ -6436,7 +6467,7 @@
         <v>-1.010373310895239E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>44469</v>
       </c>
@@ -6477,7 +6508,7 @@
         <v>2.490882073915623E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>44500</v>
       </c>
@@ -6518,7 +6549,7 @@
         <v>1.2938130031643581E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>44530</v>
       </c>
@@ -6559,7 +6590,7 @@
         <v>6.4833336615501766E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>44561</v>
       </c>
@@ -6600,7 +6631,7 @@
         <v>-9.1506380336828334E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>44592</v>
       </c>
@@ -6641,7 +6672,7 @@
         <v>-2.3824663694865631E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>44620</v>
       </c>
@@ -6682,7 +6713,7 @@
         <v>8.2846272197623257E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>44651</v>
       </c>
@@ -6723,7 +6754,7 @@
         <v>1.3036290542952299E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>44681</v>
       </c>
@@ -6764,7 +6795,7 @@
         <v>1.328423302520082E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>44712</v>
       </c>
@@ -6805,7 +6836,7 @@
         <v>-5.7001326644131817E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A155" s="3">
         <v>44742</v>
       </c>
@@ -6846,7 +6877,7 @@
         <v>-1.177606653920473E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>44773</v>
       </c>
@@ -6887,7 +6918,7 @@
         <v>-7.5656833213979899E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A157" s="3">
         <v>44804</v>
       </c>
@@ -6928,7 +6959,7 @@
         <v>5.4499286750915969E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A158" s="3">
         <v>44834</v>
       </c>
@@ -6969,7 +7000,7 @@
         <v>1.2120667261655879E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A159" s="3">
         <v>44865</v>
       </c>
@@ -7010,7 +7041,7 @@
         <v>-4.7076978575128353E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A160" s="3">
         <v>44895</v>
       </c>
@@ -7051,7 +7082,7 @@
         <v>-4.2156806117746104E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A161" s="3">
         <v>44926</v>
       </c>
@@ -7092,7 +7123,7 @@
         <v>-2.3745414668826809E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A162" s="3">
         <v>44957</v>
       </c>
@@ -7133,7 +7164,7 @@
         <v>-1.2883364518719711E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A163" s="3">
         <v>44985</v>
       </c>
@@ -7174,7 +7205,7 @@
         <v>6.4600534628154616E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A164" s="3">
         <v>45016</v>
       </c>
@@ -7215,7 +7246,7 @@
         <v>-8.9730986428309678E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A165" s="3">
         <v>45046</v>
       </c>
@@ -7256,7 +7287,7 @@
         <v>1.8527818779747009E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A166" s="3">
         <v>45077</v>
       </c>
@@ -7297,7 +7328,7 @@
         <v>-1.1140294816205641E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A167" s="3">
         <v>45107</v>
       </c>
@@ -7338,7 +7369,7 @@
         <v>-2.943892561562046E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A168" s="3">
         <v>45138</v>
       </c>
@@ -7379,7 +7410,7 @@
         <v>1.445038105123675E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A169" s="3">
         <v>45169</v>
       </c>
@@ -7414,19 +7445,76 @@
         <v>8.5543199315654128E-3</v>
       </c>
       <c r="L169" s="2">
-        <v>-1.4552965103109199E-2</v>
+        <v>-1.481990580073549E-2</v>
       </c>
       <c r="M169" s="2">
-        <v>1.999220550393721E-3</v>
+        <v>1.563584912332331E-3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A170" s="3">
+        <v>45199</v>
+      </c>
+      <c r="B170" s="2">
+        <v>-4.7677903979494229E-2</v>
+      </c>
+      <c r="C170" s="2">
+        <v>-1.902510025131765E-2</v>
+      </c>
+      <c r="D170" s="2">
+        <v>-2.288153486324163E-3</v>
+      </c>
+      <c r="E170" s="2">
+        <v>1.103157312307634E-2</v>
+      </c>
+      <c r="F170" s="2">
+        <v>5.3105252682040041E-2</v>
+      </c>
+      <c r="G170" s="2">
+        <v>-3.0100273803694839E-3</v>
+      </c>
+      <c r="H170" s="2">
+        <v>6.2609764863030826E-4</v>
+      </c>
+      <c r="I170" s="2">
+        <v>5.2094169944096004E-3</v>
+      </c>
+      <c r="J170" s="2">
+        <v>7.3804491282469797E-5</v>
+      </c>
+      <c r="K170" s="2">
+        <v>1.492790500424079E-2</v>
+      </c>
+      <c r="L170" s="2">
+        <v>-4.253836053814377E-2</v>
+      </c>
+      <c r="M170" s="2">
+        <v>7.2948358522393611E-3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A169">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+  <conditionalFormatting sqref="A1:A168">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="8">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:M169">
+  <conditionalFormatting sqref="B2:M168">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A169:A170">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A169))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B169:M170">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>